<commit_message>
change: data in tutor.xlsx and invited_code in createDatabase(Ass2_CO2013).py
</commit_message>
<xml_diff>
--- a/Dataset/tutor.xlsx
+++ b/Dataset/tutor.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="26">
   <si>
     <t>bio</t>
   </si>
@@ -181,7 +181,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -200,6 +200,9 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -644,8 +647,8 @@
       <c r="F7" s="5">
         <v>18</v>
       </c>
-      <c r="G7" s="5">
-        <v>13</v>
+      <c r="G7" s="8" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="8" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">

</xml_diff>